<commit_message>
User-Stories (Fehler behoben, letzter commit)
Co-authored-by: ynnskrnr <ynnskrnr@users.noreply.github.com>
Co-authored-by: tristanbuls <tristanbuls@users.noreply.github.com>
Co-authored-by: esrom <unigithubacc@users.noreply.github.com>
Co-authored-by: MavinScholl <MavinScholl@users.noreply.github.com>
Co-authored-by: Davipede99 <davidepedergnana99@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/project planning/User-Stories.xlsx
+++ b/project planning/User-Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Resilio Sync\Daniel Schor\Studium\Module\Aktuell\WebApp\Projekt\Repo\webappproject23-24-devteam\project planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{930E4648-6957-4379-808C-1094C0133A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0B06BEA-690E-48E5-913B-39C7A002C6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{327FAD57-2569-44E9-8BCD-A09DB2E6563B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t>Nr.</t>
   </si>
@@ -47,14 +47,125 @@
     <t>möchte ich …</t>
   </si>
   <si>
-    <t>damit/weil/denn …</t>
+    <t>Eventorganisator</t>
+  </si>
+  <si>
+    <t>Teilnehmer</t>
+  </si>
+  <si>
+    <t>eine Veranstaltung erstellen können</t>
+  </si>
+  <si>
+    <t>eine Liste der teilnehmenden Personen sehen können</t>
+  </si>
+  <si>
+    <t>Veranstaltungsstandort auf einer Karte anzeigen</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>XL</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>XS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Priorität </t>
+  </si>
+  <si>
+    <t>Veranstaltungsdetails bearbeiten können</t>
+  </si>
+  <si>
+    <t>Feedback zu einer vergangenen Veranstaltung geben</t>
+  </si>
+  <si>
+    <t>einfach nach Events suchen können</t>
+  </si>
+  <si>
+    <t>ich Veranstaltungen finde, die meinen Interessen entsprechen</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Benachrichtigung an die Teilnehmer senden können</t>
+  </si>
+  <si>
+    <t>damit/weil/denn/um …</t>
+  </si>
+  <si>
+    <t>Benutzer</t>
+  </si>
+  <si>
+    <t>mich Anmelden/Registrieren können</t>
+  </si>
+  <si>
+    <t>meine Kontoinformationen bearbeiten können</t>
+  </si>
+  <si>
+    <t>alle Events durchsuchen können</t>
+  </si>
+  <si>
+    <t>mich zu events anmelden können</t>
+  </si>
+  <si>
+    <t>Bewertungen anderer Benutzer lesen können</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ein Event im Google Kalender speichern können </t>
+  </si>
+  <si>
+    <t>mich von angemeldeten Events abmelden können</t>
+  </si>
+  <si>
+    <t>sich entscheiden zu können, ob die Veranstaltung meinen Erwartungen entspricht</t>
+  </si>
+  <si>
+    <t>die Gästeliste zu verwalten und Ressourcen zu planen</t>
+  </si>
+  <si>
+    <t>personalisierte Funktionen nutzen zu können</t>
+  </si>
+  <si>
+    <t>meine persönlichen Informationen zu aktualisieren oder zu korrigieren</t>
+  </si>
+  <si>
+    <t>auf wichtige aenderungen aufmerksam zu machen</t>
+  </si>
+  <si>
+    <t>eine visuelle Darstellung des Veranstaltungsorts zu haben</t>
+  </si>
+  <si>
+    <t>alle relevanten Informationen zu erfassen und zu organisieren</t>
+  </si>
+  <si>
+    <t>aktualisierte Informationen an die Teilnehmer weiterzugeben</t>
+  </si>
+  <si>
+    <t>den Veranstaltungstermin in meinem Kalender zu behalten</t>
+  </si>
+  <si>
+    <t>interessante Veranstaltungen zu finden</t>
+  </si>
+  <si>
+    <t>an Veranstaltungen teilzunehmen</t>
+  </si>
+  <si>
+    <t>die Qualität zukünftiger Events zu verbessern</t>
+  </si>
+  <si>
+    <t>planänderungen an den Veranstalter mitzuteilen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +178,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,14 +206,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -117,6 +241,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF5050"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -129,13 +258,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5E98E035-AE97-44B3-AFA8-6F7F6F38B269}" name="Tabelle2" displayName="Tabelle2" ref="C3:F11" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="C3:F11" xr:uid="{5E98E035-AE97-44B3-AFA8-6F7F6F38B269}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{296C035C-3354-4628-AFEB-08B0B842DC2B}" name="Nr."/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5E98E035-AE97-44B3-AFA8-6F7F6F38B269}" name="Tabelle2" displayName="Tabelle2" ref="D3:H17" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="D3:H17" xr:uid="{5E98E035-AE97-44B3-AFA8-6F7F6F38B269}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D4:H17">
+    <sortCondition ref="E3:E17"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{296C035C-3354-4628-AFEB-08B0B842DC2B}" name="Nr." dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{02F0B552-BFE9-43C0-96A8-77EDCE88AB39}" name="Als…"/>
     <tableColumn id="3" xr3:uid="{63892478-3239-4497-9AD2-245B315AE6D5}" name="möchte ich …"/>
-    <tableColumn id="4" xr3:uid="{513E1BA1-286D-4A69-A577-84390AA2B028}" name="damit/weil/denn …"/>
+    <tableColumn id="4" xr3:uid="{513E1BA1-286D-4A69-A577-84390AA2B028}" name="damit/weil/denn/um …"/>
+    <tableColumn id="5" xr3:uid="{91B42CA5-B1B9-4015-87DB-7C2C213C1DD4}" name="Priorität "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -438,32 +571,275 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B373D4FC-F6C3-49E8-AFE4-CB2A8F9188A3}">
-  <dimension ref="C3:F3"/>
+  <dimension ref="D3:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
-    <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="64.5703125" customWidth="1"/>
+    <col min="7" max="7" width="87.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="3" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
         <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D7" s="2">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="2">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="2">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="2">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D12" s="2">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D13" s="2">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D14" s="2">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D15" s="2">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D16" s="2">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D17" s="2">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>